<commit_message>
dataset2 updated for multiple regression
</commit_message>
<xml_diff>
--- a/dataset2.xlsx
+++ b/dataset2.xlsx
@@ -283,262 +283,262 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F254" sqref="F254"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">RANDBETWEEN(20, 50)</f>
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B2">
+        <f ca="1">RANDBETWEEN(1, 15)</f>
+        <v>2</v>
+      </c>
+      <c r="C2">
         <f ca="1">RANDBETWEEN(10000, 90000)</f>
-        <v>24718</v>
-      </c>
-      <c r="C2">
-        <f ca="1">RANDBETWEEN(1, 15)</f>
-        <v>10</v>
+        <v>52270</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A66" ca="1" si="0">RANDBETWEEN(20, 50)</f>
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B66" ca="1" si="1">RANDBETWEEN(10000, 90000)</f>
-        <v>75588</v>
+        <f t="shared" ref="B3:B66" ca="1" si="1">RANDBETWEEN(1, 15)</f>
+        <v>8</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C66" ca="1" si="2">RANDBETWEEN(1, 15)</f>
-        <v>15</v>
+        <f t="shared" ref="C3:C66" ca="1" si="2">RANDBETWEEN(10000, 90000)</f>
+        <v>35084</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>55146</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>15892</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>11365</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>44511</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>59975</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>10245</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>38845</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>22400</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>40354</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>76073</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>57090</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>81496</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>71359</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>54136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>78146</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>12773</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>89846</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>19651</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>78120</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>19329</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>56465</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>55259</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>13421</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>47144</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>78122</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>60796</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>49443</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>85103</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>22777</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>62403</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -548,1187 +548,1187 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>30988</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>40310</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>75920</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>58111</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>83267</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>59761</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>83269</v>
+        <v>15</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>61629</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>56313</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>41070</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>34415</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>80694</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>60209</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>65445</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>46953</v>
+        <v>13</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>81502</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>15971</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>35445</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>85557</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>13170</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>23993</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>35978</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>45685</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>21342</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>37717</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>37295</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="1"/>
-        <v>82282</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>80674</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
-        <v>56973</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>78530</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>67850</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>67057</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>34426</v>
+        <v>6</v>
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>73495</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>59288</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>59303</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>78722</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>28405</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>18750</v>
+        <v>12</v>
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>67881</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>79376</v>
+        <v>15</v>
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>53067</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>39466</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>19670</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>70731</v>
+        <v>15</v>
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>20454</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>28902</v>
+        <v>13</v>
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>32251</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>77408</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>54648</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>77601</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>34954</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>17467</v>
+        <v>11</v>
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>36837</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>29969</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>51322</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>75659</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>70369</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>33700</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>85851</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>31466</v>
+        <v>8</v>
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>17040</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>83467</v>
+        <v>11</v>
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>35752</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>52662</v>
+        <v>4</v>
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>83706</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>64814</v>
+        <v>15</v>
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>70523</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>15084</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>28948</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>11250</v>
+        <v>5</v>
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>27386</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>17531</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>22971</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>60975</v>
+        <v>14</v>
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>31945</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>67864</v>
+        <v>14</v>
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>15399</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>75992</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>13844</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>64792</v>
+        <v>7</v>
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>59357</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>76373</v>
+        <v>7</v>
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>36711</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>30912</v>
+        <v>12</v>
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>30022</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>86999</v>
+        <v>5</v>
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>67119</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>35780</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>86885</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>43697</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>68163</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>56863</v>
+        <v>14</v>
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>28731</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
-        <v>87112</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>19607</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" ref="A67:A130" ca="1" si="3">RANDBETWEEN(20, 50)</f>
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B130" ca="1" si="4">RANDBETWEEN(10000, 90000)</f>
-        <v>33074</v>
+        <f t="shared" ref="B67:B130" ca="1" si="4">RANDBETWEEN(1, 15)</f>
+        <v>12</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" ca="1" si="5">RANDBETWEEN(1, 15)</f>
-        <v>5</v>
+        <f t="shared" ref="C67:C130" ca="1" si="5">RANDBETWEEN(10000, 90000)</f>
+        <v>45824</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="4"/>
-        <v>48634</v>
+        <v>11</v>
       </c>
       <c r="C68">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>76360</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="4"/>
-        <v>74751</v>
+        <v>8</v>
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>72620</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="4"/>
-        <v>16425</v>
+        <v>14</v>
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>43516</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="4"/>
-        <v>38821</v>
+        <v>2</v>
       </c>
       <c r="C71">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>46531</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="4"/>
-        <v>28437</v>
+        <v>9</v>
       </c>
       <c r="C72">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>77533</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="4"/>
-        <v>45184</v>
+        <v>2</v>
       </c>
       <c r="C73">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>70091</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="4"/>
-        <v>75429</v>
+        <v>11</v>
       </c>
       <c r="C74">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>49870</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="4"/>
-        <v>20594</v>
+        <v>7</v>
       </c>
       <c r="C75">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>71289</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="4"/>
-        <v>41811</v>
+        <v>10</v>
       </c>
       <c r="C76">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>54353</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="4"/>
-        <v>12603</v>
+        <v>12</v>
       </c>
       <c r="C77">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>86876</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="4"/>
-        <v>12843</v>
+        <v>6</v>
       </c>
       <c r="C78">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>18599</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="4"/>
-        <v>39844</v>
+        <v>7</v>
       </c>
       <c r="C79">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>26529</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="4"/>
-        <v>24561</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>22456</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="4"/>
-        <v>45180</v>
+        <v>1</v>
       </c>
       <c r="C81">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>17421</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="4"/>
-        <v>18452</v>
+        <v>13</v>
       </c>
       <c r="C82">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>19439</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="4"/>
-        <v>29209</v>
+        <v>13</v>
       </c>
       <c r="C83">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>77171</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="4"/>
-        <v>88248</v>
+        <v>14</v>
       </c>
       <c r="C84">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>53654</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="4"/>
-        <v>36438</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>13105</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="4"/>
-        <v>78835</v>
+        <v>3</v>
       </c>
       <c r="C86">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>77098</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="4"/>
-        <v>73206</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>27070</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="4"/>
-        <v>61496</v>
+        <v>10</v>
       </c>
       <c r="C88">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>40393</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="4"/>
-        <v>85194</v>
+        <v>13</v>
       </c>
       <c r="C89">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>65008</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="4"/>
-        <v>28070</v>
+        <v>6</v>
       </c>
       <c r="C90">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>51812</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="4"/>
-        <v>23946</v>
+        <v>10</v>
       </c>
       <c r="C91">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>52077</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="4"/>
-        <v>77670</v>
+        <v>12</v>
       </c>
       <c r="C92">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>49902</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="4"/>
-        <v>70165</v>
+        <v>11</v>
       </c>
       <c r="C93">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>39692</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="4"/>
-        <v>78771</v>
+        <v>9</v>
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>64151</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="4"/>
-        <v>46710</v>
+        <v>6</v>
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>16968</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="4"/>
-        <v>47218</v>
+        <v>10</v>
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>60286</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="4"/>
-        <v>79428</v>
+        <v>5</v>
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>24362</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="4"/>
-        <v>82315</v>
+        <v>9</v>
       </c>
       <c r="C98">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>36764</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="4"/>
-        <v>59697</v>
+        <v>4</v>
       </c>
       <c r="C99">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>22894</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="4"/>
-        <v>62883</v>
+        <v>15</v>
       </c>
       <c r="C100">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>25555</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="4"/>
-        <v>25954</v>
+        <v>4</v>
       </c>
       <c r="C101">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>87950</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="4"/>
-        <v>11526</v>
+        <v>15</v>
       </c>
       <c r="C102">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>65897</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" ca="1" si="3"/>
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="4"/>
-        <v>67669</v>
+        <v>2</v>
       </c>
       <c r="C103">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>87147</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="4"/>
-        <v>21572</v>
+        <v>14</v>
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>38549</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -1752,81 +1752,81 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="4"/>
-        <v>87349</v>
+        <v>11</v>
       </c>
       <c r="C105">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>14535</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="4"/>
-        <v>62082</v>
+        <v>14</v>
       </c>
       <c r="C106">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>66593</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="4"/>
-        <v>67997</v>
+        <v>3</v>
       </c>
       <c r="C107">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>22964</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="4"/>
-        <v>82047</v>
+        <v>8</v>
       </c>
       <c r="C108">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>72520</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="4"/>
-        <v>34889</v>
+        <v>10</v>
       </c>
       <c r="C109">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>76156</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="4"/>
-        <v>63690</v>
+        <v>4</v>
       </c>
       <c r="C110">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>11107</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -1836,781 +1836,781 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="4"/>
-        <v>35000</v>
+        <v>13</v>
       </c>
       <c r="C111">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>25781</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" ca="1" si="3"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="4"/>
-        <v>66861</v>
+        <v>7</v>
       </c>
       <c r="C112">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>51963</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="4"/>
-        <v>69312</v>
+        <v>13</v>
       </c>
       <c r="C113">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>14496</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="4"/>
-        <v>14382</v>
+        <v>3</v>
       </c>
       <c r="C114">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>75931</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="4"/>
-        <v>32012</v>
+        <v>13</v>
       </c>
       <c r="C115">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>80864</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="4"/>
-        <v>31281</v>
+        <v>12</v>
       </c>
       <c r="C116">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>66175</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="4"/>
-        <v>26682</v>
+        <v>4</v>
       </c>
       <c r="C117">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>55151</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="4"/>
-        <v>79741</v>
+        <v>5</v>
       </c>
       <c r="C118">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>10152</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="4"/>
-        <v>17333</v>
+        <v>1</v>
       </c>
       <c r="C119">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>64789</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="4"/>
-        <v>78211</v>
+        <v>15</v>
       </c>
       <c r="C120">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>15158</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="4"/>
-        <v>43615</v>
+        <v>4</v>
       </c>
       <c r="C121">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>73016</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="4"/>
-        <v>72648</v>
+        <v>10</v>
       </c>
       <c r="C122">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>30285</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="4"/>
-        <v>19093</v>
+        <v>7</v>
       </c>
       <c r="C123">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>84348</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="4"/>
-        <v>78457</v>
+        <v>7</v>
       </c>
       <c r="C124">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>80650</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="4"/>
-        <v>52046</v>
+        <v>6</v>
       </c>
       <c r="C125">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>50933</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="4"/>
-        <v>45253</v>
+        <v>10</v>
       </c>
       <c r="C126">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>24955</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="4"/>
-        <v>12167</v>
+        <v>1</v>
       </c>
       <c r="C127">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>51743</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="4"/>
-        <v>86205</v>
+        <v>9</v>
       </c>
       <c r="C128">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>66411</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="4"/>
-        <v>72207</v>
+        <v>14</v>
       </c>
       <c r="C129">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>24871</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="4"/>
-        <v>21548</v>
+        <v>14</v>
       </c>
       <c r="C130">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>82445</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" ref="A131:A194" ca="1" si="6">RANDBETWEEN(20, 50)</f>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B131">
-        <f t="shared" ref="B131:B194" ca="1" si="7">RANDBETWEEN(10000, 90000)</f>
-        <v>29317</v>
+        <f t="shared" ref="B131:B194" ca="1" si="7">RANDBETWEEN(1, 15)</f>
+        <v>10</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C194" ca="1" si="8">RANDBETWEEN(1, 15)</f>
-        <v>3</v>
+        <f t="shared" ref="C131:C194" ca="1" si="8">RANDBETWEEN(10000, 90000)</f>
+        <v>70085</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="7"/>
-        <v>28183</v>
+        <v>8</v>
       </c>
       <c r="C132">
         <f t="shared" ca="1" si="8"/>
-        <v>14</v>
+        <v>20971</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" ca="1" si="6"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="7"/>
-        <v>46906</v>
+        <v>11</v>
       </c>
       <c r="C133">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>17526</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="7"/>
-        <v>89097</v>
+        <v>13</v>
       </c>
       <c r="C134">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>65162</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" ca="1" si="6"/>
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="7"/>
-        <v>49406</v>
+        <v>7</v>
       </c>
       <c r="C135">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>79261</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" ca="1" si="6"/>
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="7"/>
-        <v>83394</v>
+        <v>8</v>
       </c>
       <c r="C136">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>20121</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="7"/>
-        <v>79177</v>
+        <v>13</v>
       </c>
       <c r="C137">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>60699</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="7"/>
-        <v>64439</v>
+        <v>3</v>
       </c>
       <c r="C138">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>76679</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="7"/>
-        <v>14488</v>
+        <v>14</v>
       </c>
       <c r="C139">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>20488</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="7"/>
-        <v>34229</v>
+        <v>14</v>
       </c>
       <c r="C140">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>13582</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" ca="1" si="6"/>
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="7"/>
-        <v>78094</v>
+        <v>2</v>
       </c>
       <c r="C141">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>58265</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="7"/>
-        <v>62541</v>
+        <v>8</v>
       </c>
       <c r="C142">
         <f t="shared" ca="1" si="8"/>
-        <v>14</v>
+        <v>51552</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" ca="1" si="6"/>
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="7"/>
-        <v>57725</v>
+        <v>4</v>
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>82191</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="7"/>
-        <v>65121</v>
+        <v>15</v>
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>27720</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" ca="1" si="6"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="7"/>
-        <v>22192</v>
+        <v>13</v>
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>21348</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" ca="1" si="6"/>
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B146">
         <f t="shared" ca="1" si="7"/>
-        <v>68143</v>
+        <v>1</v>
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>35968</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" ca="1" si="6"/>
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B147">
         <f t="shared" ca="1" si="7"/>
-        <v>19403</v>
+        <v>7</v>
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>34591</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" ca="1" si="6"/>
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B148">
         <f t="shared" ca="1" si="7"/>
-        <v>53746</v>
+        <v>1</v>
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>27094</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B149">
         <f t="shared" ca="1" si="7"/>
-        <v>80508</v>
+        <v>14</v>
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>37744</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" ca="1" si="6"/>
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B150">
         <f t="shared" ca="1" si="7"/>
-        <v>61120</v>
+        <v>2</v>
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>68227</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B151">
         <f t="shared" ca="1" si="7"/>
-        <v>22847</v>
+        <v>13</v>
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>15317</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" ca="1" si="6"/>
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B152">
         <f t="shared" ca="1" si="7"/>
-        <v>24200</v>
+        <v>6</v>
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>69809</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" ca="1" si="6"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B153">
         <f t="shared" ca="1" si="7"/>
-        <v>44860</v>
+        <v>11</v>
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>20040</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B154">
         <f t="shared" ca="1" si="7"/>
-        <v>40178</v>
+        <v>13</v>
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>48924</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" ca="1" si="6"/>
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B155">
         <f t="shared" ca="1" si="7"/>
-        <v>12138</v>
+        <v>9</v>
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>46984</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B156">
         <f t="shared" ca="1" si="7"/>
-        <v>56343</v>
+        <v>12</v>
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>75571</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" ca="1" si="6"/>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B157">
         <f t="shared" ca="1" si="7"/>
-        <v>67237</v>
+        <v>3</v>
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="8"/>
-        <v>11</v>
+        <v>67646</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B158">
         <f t="shared" ca="1" si="7"/>
-        <v>37667</v>
+        <v>14</v>
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>50526</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" ca="1" si="6"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B159">
         <f t="shared" ca="1" si="7"/>
-        <v>11953</v>
+        <v>13</v>
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>18955</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B160">
         <f t="shared" ca="1" si="7"/>
-        <v>64314</v>
+        <v>8</v>
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>20212</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161">
         <f t="shared" ca="1" si="6"/>
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B161">
         <f t="shared" ca="1" si="7"/>
-        <v>83002</v>
+        <v>4</v>
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>84130</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" ca="1" si="6"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B162">
         <f t="shared" ca="1" si="7"/>
-        <v>22362</v>
+        <v>13</v>
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>57526</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" ca="1" si="6"/>
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B163">
         <f t="shared" ca="1" si="7"/>
-        <v>21994</v>
+        <v>7</v>
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>65369</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B164">
         <f t="shared" ca="1" si="7"/>
-        <v>57519</v>
+        <v>15</v>
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>37952</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B165">
         <f t="shared" ca="1" si="7"/>
-        <v>40869</v>
+        <v>3</v>
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>53136</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B166">
         <f t="shared" ca="1" si="7"/>
-        <v>51745</v>
+        <v>11</v>
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>25226</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -2620,221 +2620,221 @@
       </c>
       <c r="B167">
         <f t="shared" ca="1" si="7"/>
-        <v>50621</v>
+        <v>9</v>
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>78828</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
         <f t="shared" ca="1" si="6"/>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B168">
         <f t="shared" ca="1" si="7"/>
-        <v>32784</v>
+        <v>3</v>
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>69138</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
         <f t="shared" ca="1" si="6"/>
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B169">
         <f t="shared" ca="1" si="7"/>
-        <v>67713</v>
+        <v>8</v>
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>34154</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B170">
         <f t="shared" ca="1" si="7"/>
-        <v>40275</v>
+        <v>12</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>73660</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B171">
         <f t="shared" ca="1" si="7"/>
-        <v>67251</v>
+        <v>15</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>42606</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B172">
         <f t="shared" ca="1" si="7"/>
-        <v>47705</v>
+        <v>8</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>36772</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
         <f t="shared" ca="1" si="6"/>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B173">
         <f t="shared" ca="1" si="7"/>
-        <v>23137</v>
+        <v>11</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>86523</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B174">
         <f t="shared" ca="1" si="7"/>
-        <v>81875</v>
+        <v>6</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>35581</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175">
         <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B175">
         <f t="shared" ca="1" si="7"/>
-        <v>76583</v>
+        <v>6</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>22064</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B176">
         <f t="shared" ca="1" si="7"/>
-        <v>82238</v>
+        <v>15</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="8"/>
-        <v>11</v>
+        <v>43687</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
         <f t="shared" ca="1" si="6"/>
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B177">
         <f t="shared" ca="1" si="7"/>
-        <v>26754</v>
+        <v>12</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>68671</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
         <f t="shared" ca="1" si="6"/>
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B178">
         <f t="shared" ca="1" si="7"/>
-        <v>55829</v>
+        <v>14</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>48730</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
         <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B179">
         <f t="shared" ca="1" si="7"/>
-        <v>11848</v>
+        <v>10</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="8"/>
-        <v>14</v>
+        <v>38389</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
         <f t="shared" ca="1" si="6"/>
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B180">
         <f t="shared" ca="1" si="7"/>
-        <v>23412</v>
+        <v>10</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>24353</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
         <f t="shared" ca="1" si="6"/>
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B181">
         <f t="shared" ca="1" si="7"/>
-        <v>31069</v>
+        <v>2</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>88836</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B182">
         <f t="shared" ca="1" si="7"/>
-        <v>87542</v>
+        <v>10</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>11044</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
@@ -2844,95 +2844,95 @@
       </c>
       <c r="B183">
         <f t="shared" ca="1" si="7"/>
-        <v>33706</v>
+        <v>4</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>32259</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B184">
         <f t="shared" ca="1" si="7"/>
-        <v>32265</v>
+        <v>12</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>82556</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B185">
         <f t="shared" ca="1" si="7"/>
-        <v>52219</v>
+        <v>4</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>64339</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186">
         <f t="shared" ca="1" si="6"/>
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B186">
         <f t="shared" ca="1" si="7"/>
-        <v>74739</v>
+        <v>1</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>18786</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187">
         <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B187">
         <f t="shared" ca="1" si="7"/>
-        <v>31371</v>
+        <v>4</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>37037</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
         <f t="shared" ca="1" si="6"/>
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B188">
         <f t="shared" ca="1" si="7"/>
-        <v>68369</v>
+        <v>7</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>56068</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
         <f t="shared" ca="1" si="6"/>
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B189">
         <f t="shared" ca="1" si="7"/>
-        <v>30372</v>
+        <v>13</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>60009</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -2942,11 +2942,11 @@
       </c>
       <c r="B190">
         <f t="shared" ca="1" si="7"/>
-        <v>39232</v>
+        <v>2</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>87313</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -2956,431 +2956,431 @@
       </c>
       <c r="B191">
         <f t="shared" ca="1" si="7"/>
-        <v>45637</v>
+        <v>2</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>22185</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B192">
         <f t="shared" ca="1" si="7"/>
-        <v>73893</v>
+        <v>3</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>13710</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193">
         <f t="shared" ca="1" si="6"/>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B193">
         <f t="shared" ca="1" si="7"/>
-        <v>39630</v>
+        <v>8</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>47644</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194">
         <f t="shared" ca="1" si="6"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B194">
         <f t="shared" ca="1" si="7"/>
-        <v>28032</v>
+        <v>9</v>
       </c>
       <c r="C194">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>39322</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195">
         <f t="shared" ref="A195:A256" ca="1" si="9">RANDBETWEEN(20, 50)</f>
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B195">
-        <f t="shared" ref="B195:B257" ca="1" si="10">RANDBETWEEN(10000, 90000)</f>
-        <v>70746</v>
+        <f t="shared" ref="B195:B257" ca="1" si="10">RANDBETWEEN(1, 15)</f>
+        <v>7</v>
       </c>
       <c r="C195">
-        <f t="shared" ref="C195:C257" ca="1" si="11">RANDBETWEEN(1, 15)</f>
-        <v>11</v>
+        <f t="shared" ref="C195:C257" ca="1" si="11">RANDBETWEEN(10000, 90000)</f>
+        <v>63898</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196">
         <f t="shared" ca="1" si="9"/>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="10"/>
-        <v>59638</v>
+        <v>5</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>16184</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197">
         <f t="shared" ca="1" si="9"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="10"/>
-        <v>62053</v>
+        <v>10</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="11"/>
-        <v>7</v>
+        <v>72535</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198">
         <f t="shared" ca="1" si="9"/>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="10"/>
-        <v>62580</v>
+        <v>11</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="11"/>
-        <v>11</v>
+        <v>12117</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199">
         <f t="shared" ca="1" si="9"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="10"/>
-        <v>64111</v>
+        <v>2</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="11"/>
-        <v>6</v>
+        <v>24523</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200">
         <f t="shared" ca="1" si="9"/>
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="10"/>
-        <v>15508</v>
+        <v>2</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>74702</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201">
         <f t="shared" ca="1" si="9"/>
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="10"/>
-        <v>66149</v>
+        <v>9</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="11"/>
-        <v>6</v>
+        <v>66282</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202">
         <f t="shared" ca="1" si="9"/>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="10"/>
-        <v>13971</v>
+        <v>1</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>32396</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203">
         <f t="shared" ca="1" si="9"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="10"/>
-        <v>39887</v>
+        <v>7</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="11"/>
-        <v>10</v>
+        <v>73368</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204">
         <f t="shared" ca="1" si="9"/>
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="10"/>
-        <v>24140</v>
+        <v>4</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>23229</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205">
         <f t="shared" ca="1" si="9"/>
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="10"/>
-        <v>14582</v>
+        <v>1</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>89495</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206">
         <f t="shared" ca="1" si="9"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="10"/>
-        <v>39540</v>
+        <v>9</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>56416</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207">
         <f t="shared" ca="1" si="9"/>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="10"/>
-        <v>80833</v>
+        <v>8</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>61844</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208">
         <f t="shared" ca="1" si="9"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="10"/>
-        <v>56256</v>
+        <v>3</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>32831</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209">
         <f t="shared" ca="1" si="9"/>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="10"/>
-        <v>15092</v>
+        <v>8</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="11"/>
-        <v>11</v>
+        <v>83432</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210">
         <f t="shared" ca="1" si="9"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="10"/>
-        <v>61244</v>
+        <v>15</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="11"/>
-        <v>12</v>
+        <v>28099</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211">
         <f t="shared" ca="1" si="9"/>
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="10"/>
-        <v>82148</v>
+        <v>11</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>10521</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212">
         <f t="shared" ca="1" si="9"/>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="10"/>
-        <v>63004</v>
+        <v>5</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213">
         <f t="shared" ca="1" si="9"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="10"/>
-        <v>15587</v>
+        <v>9</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="11"/>
-        <v>10</v>
+        <v>23171</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214">
         <f t="shared" ca="1" si="9"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="10"/>
-        <v>57286</v>
+        <v>6</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="11"/>
-        <v>10</v>
+        <v>40664</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215">
         <f t="shared" ca="1" si="9"/>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B215">
         <f t="shared" ca="1" si="10"/>
-        <v>14072</v>
+        <v>5</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="11"/>
-        <v>12</v>
+        <v>85759</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216">
         <f t="shared" ca="1" si="9"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B216">
         <f t="shared" ca="1" si="10"/>
-        <v>28943</v>
+        <v>8</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>43588</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217">
         <f t="shared" ca="1" si="9"/>
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B217">
         <f t="shared" ca="1" si="10"/>
-        <v>66404</v>
+        <v>15</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
+        <v>57960</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218">
         <f t="shared" ca="1" si="9"/>
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B218">
         <f t="shared" ca="1" si="10"/>
-        <v>77593</v>
+        <v>4</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>26707</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219">
         <f t="shared" ca="1" si="9"/>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B219">
         <f t="shared" ca="1" si="10"/>
-        <v>29483</v>
+        <v>2</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>62778</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220">
         <f t="shared" ca="1" si="9"/>
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B220">
         <f t="shared" ca="1" si="10"/>
-        <v>78527</v>
+        <v>14</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>45408</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221">
         <f t="shared" ca="1" si="9"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B221">
         <f t="shared" ca="1" si="10"/>
-        <v>14058</v>
+        <v>2</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>48717</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
@@ -3390,25 +3390,25 @@
       </c>
       <c r="B222">
         <f t="shared" ca="1" si="10"/>
-        <v>39476</v>
+        <v>4</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="11"/>
-        <v>11</v>
+        <v>89262</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223">
         <f t="shared" ca="1" si="9"/>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B223">
         <f t="shared" ca="1" si="10"/>
-        <v>75032</v>
+        <v>9</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
+        <v>76691</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
@@ -3418,67 +3418,67 @@
       </c>
       <c r="B224">
         <f t="shared" ca="1" si="10"/>
-        <v>19562</v>
+        <v>2</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
+        <v>21389</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225">
         <f t="shared" ca="1" si="9"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B225">
         <f t="shared" ca="1" si="10"/>
-        <v>30253</v>
+        <v>14</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>14227</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226">
         <f t="shared" ca="1" si="9"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B226">
         <f t="shared" ca="1" si="10"/>
-        <v>78678</v>
+        <v>3</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="11"/>
-        <v>15</v>
+        <v>81374</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227">
         <f t="shared" ca="1" si="9"/>
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B227">
         <f t="shared" ca="1" si="10"/>
-        <v>37126</v>
+        <v>8</v>
       </c>
       <c r="C227">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>41239</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228">
         <f t="shared" ca="1" si="9"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B228">
         <f t="shared" ca="1" si="10"/>
-        <v>87676</v>
+        <v>15</v>
       </c>
       <c r="C228">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
+        <v>35853</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
@@ -3488,151 +3488,151 @@
       </c>
       <c r="B229">
         <f t="shared" ca="1" si="10"/>
-        <v>16821</v>
+        <v>12</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="11"/>
-        <v>9</v>
+        <v>60811</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230">
         <f t="shared" ca="1" si="9"/>
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B230">
         <f t="shared" ca="1" si="10"/>
-        <v>33315</v>
+        <v>14</v>
       </c>
       <c r="C230">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>41691</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231">
         <f t="shared" ca="1" si="9"/>
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B231">
         <f t="shared" ca="1" si="10"/>
-        <v>47830</v>
+        <v>13</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>26157</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232">
         <f t="shared" ca="1" si="9"/>
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B232">
         <f t="shared" ca="1" si="10"/>
-        <v>22792</v>
+        <v>2</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
+        <v>84663</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233">
         <f t="shared" ca="1" si="9"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B233">
         <f t="shared" ca="1" si="10"/>
-        <v>48821</v>
+        <v>2</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="11"/>
-        <v>10</v>
+        <v>75886</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234">
         <f t="shared" ca="1" si="9"/>
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B234">
         <f t="shared" ca="1" si="10"/>
-        <v>35055</v>
+        <v>13</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="11"/>
-        <v>12</v>
+        <v>64933</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235">
         <f t="shared" ca="1" si="9"/>
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B235">
         <f t="shared" ca="1" si="10"/>
-        <v>16214</v>
+        <v>15</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="11"/>
-        <v>13</v>
+        <v>49396</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236">
         <f t="shared" ca="1" si="9"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B236">
         <f t="shared" ca="1" si="10"/>
-        <v>24882</v>
+        <v>3</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>73104</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237">
         <f t="shared" ca="1" si="9"/>
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B237">
         <f t="shared" ca="1" si="10"/>
-        <v>55978</v>
+        <v>4</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>80552</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238">
         <f t="shared" ca="1" si="9"/>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B238">
         <f t="shared" ca="1" si="10"/>
-        <v>47918</v>
+        <v>13</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>68459</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239">
         <f t="shared" ca="1" si="9"/>
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B239">
         <f t="shared" ca="1" si="10"/>
-        <v>32757</v>
+        <v>8</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="11"/>
-        <v>13</v>
+        <v>18140</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
@@ -3642,67 +3642,67 @@
       </c>
       <c r="B240">
         <f t="shared" ca="1" si="10"/>
-        <v>64061</v>
+        <v>3</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>72563</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
         <f t="shared" ca="1" si="9"/>
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B241">
         <f t="shared" ca="1" si="10"/>
-        <v>33091</v>
+        <v>5</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>41906</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
         <f t="shared" ca="1" si="9"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B242">
         <f t="shared" ca="1" si="10"/>
-        <v>38648</v>
+        <v>15</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>81816</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
         <f t="shared" ca="1" si="9"/>
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B243">
         <f t="shared" ca="1" si="10"/>
-        <v>41012</v>
+        <v>9</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>49829</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
         <f t="shared" ca="1" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B244">
         <f t="shared" ca="1" si="10"/>
-        <v>23932</v>
+        <v>9</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="11"/>
-        <v>15</v>
+        <v>17125</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
@@ -3712,53 +3712,53 @@
       </c>
       <c r="B245">
         <f t="shared" ca="1" si="10"/>
-        <v>82258</v>
+        <v>2</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>48584</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
         <f t="shared" ca="1" si="9"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B246">
         <f t="shared" ca="1" si="10"/>
-        <v>56495</v>
+        <v>6</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="11"/>
-        <v>10</v>
+        <v>17883</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
         <f t="shared" ca="1" si="9"/>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B247">
         <f t="shared" ca="1" si="10"/>
-        <v>47583</v>
+        <v>6</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="11"/>
-        <v>13</v>
+        <v>34078</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248">
         <f t="shared" ca="1" si="9"/>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B248">
         <f t="shared" ca="1" si="10"/>
-        <v>82843</v>
+        <v>3</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
+        <v>42699</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -3768,95 +3768,95 @@
       </c>
       <c r="B249">
         <f t="shared" ca="1" si="10"/>
-        <v>26640</v>
+        <v>3</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="11"/>
-        <v>6</v>
+        <v>28486</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250">
         <f t="shared" ca="1" si="9"/>
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B250">
         <f t="shared" ca="1" si="10"/>
-        <v>79963</v>
+        <v>4</v>
       </c>
       <c r="C250">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>63376</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251">
         <f t="shared" ca="1" si="9"/>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B251">
         <f t="shared" ca="1" si="10"/>
-        <v>69548</v>
+        <v>13</v>
       </c>
       <c r="C251">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
+        <v>47245</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252">
         <f t="shared" ca="1" si="9"/>
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B252">
         <f t="shared" ca="1" si="10"/>
-        <v>71260</v>
+        <v>2</v>
       </c>
       <c r="C252">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
+        <v>26136</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253">
         <f t="shared" ca="1" si="9"/>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B253">
         <f t="shared" ca="1" si="10"/>
-        <v>21784</v>
+        <v>2</v>
       </c>
       <c r="C253">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>12504</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254">
         <f t="shared" ca="1" si="9"/>
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B254">
         <f t="shared" ca="1" si="10"/>
-        <v>78813</v>
+        <v>13</v>
       </c>
       <c r="C254">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>33942</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255">
         <f t="shared" ca="1" si="9"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B255">
         <f t="shared" ca="1" si="10"/>
-        <v>26656</v>
+        <v>2</v>
       </c>
       <c r="C255">
         <f t="shared" ca="1" si="11"/>
-        <v>8</v>
+        <v>84823</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
@@ -3866,25 +3866,25 @@
       </c>
       <c r="B256">
         <f t="shared" ca="1" si="10"/>
-        <v>35744</v>
+        <v>5</v>
       </c>
       <c r="C256">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>46878</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
-        <f t="shared" ref="A195:A257" ca="1" si="12">RANDBETWEEN(1, 50)</f>
-        <v>42</v>
+        <f t="shared" ref="A257" ca="1" si="12">RANDBETWEEN(1, 50)</f>
+        <v>28</v>
       </c>
       <c r="B257">
         <f t="shared" ca="1" si="10"/>
-        <v>63380</v>
+        <v>8</v>
       </c>
       <c r="C257">
         <f t="shared" ca="1" si="11"/>
-        <v>13</v>
+        <v>21478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>